<commit_message>
rebuilding site Wed Oct  4 21:37:00 CEST 2017
</commit_message>
<xml_diff>
--- a/verb-list.xlsx
+++ b/verb-list.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/therimalaya/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/therimalaya/Dropbox/Courses/NorskKurs/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="8600" yWindow="3160" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="FraNoenWebSide" sheetId="1" r:id="rId1"/>
@@ -5807,11 +5807,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:G379"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G248" sqref="G248"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5847,7 +5846,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5867,7 +5866,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -5887,7 +5886,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -5907,7 +5906,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -5927,7 +5926,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -5947,7 +5946,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -5967,7 +5966,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -5987,7 +5986,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -6007,7 +6006,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -6027,7 +6026,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1</v>
       </c>
@@ -6050,7 +6049,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1</v>
       </c>
@@ -6070,7 +6069,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1</v>
       </c>
@@ -6090,7 +6089,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1</v>
       </c>
@@ -6110,7 +6109,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1</v>
       </c>
@@ -6130,7 +6129,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1</v>
       </c>
@@ -6150,7 +6149,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1</v>
       </c>
@@ -6170,7 +6169,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1</v>
       </c>
@@ -6190,7 +6189,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1</v>
       </c>
@@ -6210,7 +6209,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1</v>
       </c>
@@ -6230,7 +6229,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1</v>
       </c>
@@ -6250,7 +6249,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1</v>
       </c>
@@ -6270,7 +6269,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1</v>
       </c>
@@ -6290,7 +6289,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1</v>
       </c>
@@ -6310,7 +6309,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>1</v>
       </c>
@@ -6330,7 +6329,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1</v>
       </c>
@@ -6350,7 +6349,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>1</v>
       </c>
@@ -6373,7 +6372,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1</v>
       </c>
@@ -6393,7 +6392,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1</v>
       </c>
@@ -6413,7 +6412,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1</v>
       </c>
@@ -6433,7 +6432,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1</v>
       </c>
@@ -6453,7 +6452,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>1</v>
       </c>
@@ -6476,7 +6475,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>1</v>
       </c>
@@ -6496,7 +6495,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>1</v>
       </c>
@@ -6516,7 +6515,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>1</v>
       </c>
@@ -6536,7 +6535,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>1</v>
       </c>
@@ -6559,7 +6558,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="37" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>1</v>
       </c>
@@ -6582,7 +6581,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>1</v>
       </c>
@@ -6605,7 +6604,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>1</v>
       </c>
@@ -6625,7 +6624,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>1</v>
       </c>
@@ -6648,7 +6647,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>1</v>
       </c>
@@ -6671,7 +6670,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>1</v>
       </c>
@@ -6691,7 +6690,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>1</v>
       </c>
@@ -6711,7 +6710,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>1</v>
       </c>
@@ -6731,7 +6730,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>1</v>
       </c>
@@ -6751,7 +6750,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>1</v>
       </c>
@@ -6771,7 +6770,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>1</v>
       </c>
@@ -6794,7 +6793,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>1</v>
       </c>
@@ -6814,7 +6813,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="49" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>1</v>
       </c>
@@ -6834,7 +6833,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="50" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>1</v>
       </c>
@@ -6854,7 +6853,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="51" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>1</v>
       </c>
@@ -6874,7 +6873,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>1</v>
       </c>
@@ -6897,7 +6896,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="53" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>1</v>
       </c>
@@ -6917,7 +6916,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>1</v>
       </c>
@@ -6937,7 +6936,7 @@
         <v>938</v>
       </c>
     </row>
-    <row r="55" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>1</v>
       </c>
@@ -6960,7 +6959,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>1</v>
       </c>
@@ -6980,7 +6979,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="57" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>1</v>
       </c>
@@ -7000,7 +6999,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="58" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>1</v>
       </c>
@@ -7017,7 +7016,7 @@
         <v>974</v>
       </c>
     </row>
-    <row r="59" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>1</v>
       </c>
@@ -7037,7 +7036,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="60" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>1</v>
       </c>
@@ -7057,7 +7056,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="61" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>1</v>
       </c>
@@ -7080,7 +7079,7 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="62" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>1</v>
       </c>
@@ -7100,7 +7099,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="63" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>1</v>
       </c>
@@ -7120,7 +7119,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="64" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>1</v>
       </c>
@@ -7140,7 +7139,7 @@
         <v>1063</v>
       </c>
     </row>
-    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>1</v>
       </c>
@@ -7160,7 +7159,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>1</v>
       </c>
@@ -7180,7 +7179,7 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="67" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>1</v>
       </c>
@@ -7200,7 +7199,7 @@
         <v>1113</v>
       </c>
     </row>
-    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>1</v>
       </c>
@@ -7220,7 +7219,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="69" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>1</v>
       </c>
@@ -7240,7 +7239,7 @@
         <v>1123</v>
       </c>
     </row>
-    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>1</v>
       </c>
@@ -7263,7 +7262,7 @@
         <v>1138</v>
       </c>
     </row>
-    <row r="71" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>1</v>
       </c>
@@ -7286,7 +7285,7 @@
         <v>1155</v>
       </c>
     </row>
-    <row r="72" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>1</v>
       </c>
@@ -7309,7 +7308,7 @@
         <v>1178</v>
       </c>
     </row>
-    <row r="73" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>1</v>
       </c>
@@ -7329,7 +7328,7 @@
         <v>1172</v>
       </c>
     </row>
-    <row r="74" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>1</v>
       </c>
@@ -7349,7 +7348,7 @@
         <v>1218</v>
       </c>
     </row>
-    <row r="75" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>1</v>
       </c>
@@ -7369,7 +7368,7 @@
         <v>1223</v>
       </c>
     </row>
-    <row r="76" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>1</v>
       </c>
@@ -7389,7 +7388,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="77" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>1</v>
       </c>
@@ -7409,7 +7408,7 @@
         <v>1306</v>
       </c>
     </row>
-    <row r="78" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>1</v>
       </c>
@@ -7429,7 +7428,7 @@
         <v>1325</v>
       </c>
     </row>
-    <row r="79" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>1</v>
       </c>
@@ -7449,7 +7448,7 @@
         <v>1358</v>
       </c>
     </row>
-    <row r="80" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>1</v>
       </c>
@@ -7469,7 +7468,7 @@
         <v>1363</v>
       </c>
     </row>
-    <row r="81" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>1</v>
       </c>
@@ -7492,7 +7491,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="82" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>1</v>
       </c>
@@ -7515,7 +7514,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="83" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>1</v>
       </c>
@@ -7535,7 +7534,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="84" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>1</v>
       </c>
@@ -7555,7 +7554,7 @@
         <v>1445</v>
       </c>
     </row>
-    <row r="85" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>1</v>
       </c>
@@ -7575,7 +7574,7 @@
         <v>1473</v>
       </c>
     </row>
-    <row r="86" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>1</v>
       </c>
@@ -7595,7 +7594,7 @@
         <v>1478</v>
       </c>
     </row>
-    <row r="87" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>1</v>
       </c>
@@ -7615,7 +7614,7 @@
         <v>1483</v>
       </c>
     </row>
-    <row r="88" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>1</v>
       </c>
@@ -7635,7 +7634,7 @@
         <v>1501</v>
       </c>
     </row>
-    <row r="89" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>1</v>
       </c>
@@ -7655,7 +7654,7 @@
         <v>1535</v>
       </c>
     </row>
-    <row r="90" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>1</v>
       </c>
@@ -7675,7 +7674,7 @@
         <v>1546</v>
       </c>
     </row>
-    <row r="91" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>1</v>
       </c>
@@ -7695,7 +7694,7 @@
         <v>1564</v>
       </c>
     </row>
-    <row r="92" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>1</v>
       </c>
@@ -7715,7 +7714,7 @@
         <v>1569</v>
       </c>
     </row>
-    <row r="93" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>1</v>
       </c>
@@ -7735,7 +7734,7 @@
         <v>1598</v>
       </c>
     </row>
-    <row r="94" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>1</v>
       </c>
@@ -7755,7 +7754,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="95" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>1</v>
       </c>
@@ -7775,7 +7774,7 @@
         <v>1583</v>
       </c>
     </row>
-    <row r="96" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>1</v>
       </c>
@@ -7795,7 +7794,7 @@
         <v>1630</v>
       </c>
     </row>
-    <row r="97" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>1</v>
       </c>
@@ -7815,7 +7814,7 @@
         <v>1645</v>
       </c>
     </row>
-    <row r="98" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>1</v>
       </c>
@@ -7835,7 +7834,7 @@
         <v>1655</v>
       </c>
     </row>
-    <row r="99" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>1</v>
       </c>
@@ -7855,7 +7854,7 @@
         <v>1669</v>
       </c>
     </row>
-    <row r="100" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>1</v>
       </c>
@@ -7875,7 +7874,7 @@
         <v>1674</v>
       </c>
     </row>
-    <row r="101" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>1</v>
       </c>
@@ -7895,7 +7894,7 @@
         <v>1705</v>
       </c>
     </row>
-    <row r="102" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>1</v>
       </c>
@@ -7915,7 +7914,7 @@
         <v>1710</v>
       </c>
     </row>
-    <row r="103" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>1</v>
       </c>
@@ -7935,7 +7934,7 @@
         <v>1719</v>
       </c>
     </row>
-    <row r="104" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>1</v>
       </c>
@@ -7955,7 +7954,7 @@
         <v>1778</v>
       </c>
     </row>
-    <row r="105" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>1</v>
       </c>
@@ -7975,7 +7974,7 @@
         <v>1788</v>
       </c>
     </row>
-    <row r="106" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>1</v>
       </c>
@@ -7995,7 +7994,7 @@
         <v>1811</v>
       </c>
     </row>
-    <row r="107" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>2</v>
       </c>
@@ -8018,7 +8017,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="108" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>2</v>
       </c>
@@ -8041,7 +8040,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="109" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>2</v>
       </c>
@@ -8061,7 +8060,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="110" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>2</v>
       </c>
@@ -8081,7 +8080,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="111" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>2</v>
       </c>
@@ -8101,7 +8100,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="112" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>2</v>
       </c>
@@ -8121,7 +8120,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="113" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>2</v>
       </c>
@@ -8141,7 +8140,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="114" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>2</v>
       </c>
@@ -8161,7 +8160,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="115" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>2</v>
       </c>
@@ -8181,7 +8180,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="116" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>2</v>
       </c>
@@ -8201,7 +8200,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="117" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>2</v>
       </c>
@@ -8224,7 +8223,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="118" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>2</v>
       </c>
@@ -8244,7 +8243,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="119" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>2</v>
       </c>
@@ -8264,7 +8263,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="120" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>2</v>
       </c>
@@ -8287,7 +8286,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="121" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>2</v>
       </c>
@@ -8307,7 +8306,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="122" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>2</v>
       </c>
@@ -8327,7 +8326,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="123" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>2</v>
       </c>
@@ -8347,7 +8346,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="124" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>2</v>
       </c>
@@ -8367,7 +8366,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="125" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>2</v>
       </c>
@@ -8387,7 +8386,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="126" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>2</v>
       </c>
@@ -8407,7 +8406,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="127" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>2</v>
       </c>
@@ -8427,7 +8426,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="128" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>2</v>
       </c>
@@ -8447,7 +8446,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="129" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>2</v>
       </c>
@@ -8467,7 +8466,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="130" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>2</v>
       </c>
@@ -8487,7 +8486,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="131" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>2</v>
       </c>
@@ -8507,7 +8506,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="132" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>2</v>
       </c>
@@ -8527,7 +8526,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="133" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>2</v>
       </c>
@@ -8550,7 +8549,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="134" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>2</v>
       </c>
@@ -8570,7 +8569,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="135" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>2</v>
       </c>
@@ -8590,7 +8589,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="136" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>2</v>
       </c>
@@ -8610,7 +8609,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="137" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>2</v>
       </c>
@@ -8630,7 +8629,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="138" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>2</v>
       </c>
@@ -8650,7 +8649,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="139" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>2</v>
       </c>
@@ -8670,7 +8669,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="140" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>2</v>
       </c>
@@ -8690,7 +8689,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="141" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>2</v>
       </c>
@@ -8710,7 +8709,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="142" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>2</v>
       </c>
@@ -8730,7 +8729,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="143" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>2</v>
       </c>
@@ -8750,7 +8749,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="144" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>2</v>
       </c>
@@ -8770,7 +8769,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="145" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>2</v>
       </c>
@@ -8790,7 +8789,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="146" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>2</v>
       </c>
@@ -8810,7 +8809,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="147" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>2</v>
       </c>
@@ -8830,7 +8829,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="148" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>2</v>
       </c>
@@ -8850,7 +8849,7 @@
         <v>889</v>
       </c>
     </row>
-    <row r="149" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>2</v>
       </c>
@@ -8870,7 +8869,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="150" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>2</v>
       </c>
@@ -8890,7 +8889,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="151" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>2</v>
       </c>
@@ -8910,7 +8909,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="152" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>2</v>
       </c>
@@ -8930,7 +8929,7 @@
         <v>947</v>
       </c>
     </row>
-    <row r="153" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>2</v>
       </c>
@@ -8950,7 +8949,7 @@
         <v>951</v>
       </c>
     </row>
-    <row r="154" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>2</v>
       </c>
@@ -8970,7 +8969,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="155" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>2</v>
       </c>
@@ -8990,7 +8989,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="156" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>2</v>
       </c>
@@ -9010,7 +9009,7 @@
         <v>991</v>
       </c>
     </row>
-    <row r="157" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>2</v>
       </c>
@@ -9030,7 +9029,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="158" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>2</v>
       </c>
@@ -9050,7 +9049,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="159" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>2</v>
       </c>
@@ -9070,7 +9069,7 @@
         <v>1034</v>
       </c>
     </row>
-    <row r="160" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>2</v>
       </c>
@@ -9090,7 +9089,7 @@
         <v>1058</v>
       </c>
     </row>
-    <row r="161" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>2</v>
       </c>
@@ -9110,7 +9109,7 @@
         <v>1072</v>
       </c>
     </row>
-    <row r="162" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>2</v>
       </c>
@@ -9130,7 +9129,7 @@
         <v>1076</v>
       </c>
     </row>
-    <row r="163" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>2</v>
       </c>
@@ -9150,7 +9149,7 @@
         <v>1080</v>
       </c>
     </row>
-    <row r="164" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>2</v>
       </c>
@@ -9170,7 +9169,7 @@
         <v>1084</v>
       </c>
     </row>
-    <row r="165" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>2</v>
       </c>
@@ -9190,7 +9189,7 @@
         <v>1089</v>
       </c>
     </row>
-    <row r="166" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>2</v>
       </c>
@@ -9210,7 +9209,7 @@
         <v>1108</v>
       </c>
     </row>
-    <row r="167" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>2</v>
       </c>
@@ -9230,7 +9229,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="168" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>2</v>
       </c>
@@ -9250,7 +9249,7 @@
         <v>1159</v>
       </c>
     </row>
-    <row r="169" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>2</v>
       </c>
@@ -9270,7 +9269,7 @@
         <v>1163</v>
       </c>
     </row>
-    <row r="170" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>2</v>
       </c>
@@ -9290,7 +9289,7 @@
         <v>1167</v>
       </c>
     </row>
-    <row r="171" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>2</v>
       </c>
@@ -9310,7 +9309,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="172" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>2</v>
       </c>
@@ -9333,7 +9332,7 @@
         <v>1190</v>
       </c>
     </row>
-    <row r="173" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>2</v>
       </c>
@@ -9353,7 +9352,7 @@
         <v>1194</v>
       </c>
     </row>
-    <row r="174" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>2</v>
       </c>
@@ -9373,7 +9372,7 @@
         <v>1198</v>
       </c>
     </row>
-    <row r="175" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>2</v>
       </c>
@@ -9393,7 +9392,7 @@
         <v>1202</v>
       </c>
     </row>
-    <row r="176" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>2</v>
       </c>
@@ -9416,7 +9415,7 @@
         <v>1243</v>
       </c>
     </row>
-    <row r="177" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>2</v>
       </c>
@@ -9436,7 +9435,7 @@
         <v>1251</v>
       </c>
     </row>
-    <row r="178" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>2</v>
       </c>
@@ -9456,7 +9455,7 @@
         <v>1301</v>
       </c>
     </row>
-    <row r="179" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>2</v>
       </c>
@@ -9476,7 +9475,7 @@
         <v>1339</v>
       </c>
     </row>
-    <row r="180" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>2</v>
       </c>
@@ -9499,7 +9498,7 @@
         <v>1353</v>
       </c>
     </row>
-    <row r="181" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>2</v>
       </c>
@@ -9519,7 +9518,7 @@
         <v>1367</v>
       </c>
     </row>
-    <row r="182" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>2</v>
       </c>
@@ -9539,7 +9538,7 @@
         <v>1371</v>
       </c>
     </row>
-    <row r="183" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>2</v>
       </c>
@@ -9562,7 +9561,7 @@
         <v>1381</v>
       </c>
     </row>
-    <row r="184" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>2</v>
       </c>
@@ -9582,7 +9581,7 @@
         <v>1385</v>
       </c>
     </row>
-    <row r="185" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>2</v>
       </c>
@@ -9602,7 +9601,7 @@
         <v>1409</v>
       </c>
     </row>
-    <row r="186" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>2</v>
       </c>
@@ -9625,7 +9624,7 @@
         <v>1426</v>
       </c>
     </row>
-    <row r="187" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>2</v>
       </c>
@@ -9648,7 +9647,7 @@
         <v>1431</v>
       </c>
     </row>
-    <row r="188" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>2</v>
       </c>
@@ -9668,7 +9667,7 @@
         <v>1468</v>
       </c>
     </row>
-    <row r="189" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>2</v>
       </c>
@@ -9688,7 +9687,7 @@
         <v>1487</v>
       </c>
     </row>
-    <row r="190" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>2</v>
       </c>
@@ -9711,7 +9710,7 @@
         <v>1511</v>
       </c>
     </row>
-    <row r="191" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A191">
         <v>2</v>
       </c>
@@ -9731,7 +9730,7 @@
         <v>1525</v>
       </c>
     </row>
-    <row r="192" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>2</v>
       </c>
@@ -9751,7 +9750,7 @@
         <v>1550</v>
       </c>
     </row>
-    <row r="193" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>2</v>
       </c>
@@ -9774,7 +9773,7 @@
         <v>1579</v>
       </c>
     </row>
-    <row r="194" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>2</v>
       </c>
@@ -9794,7 +9793,7 @@
         <v>1608</v>
       </c>
     </row>
-    <row r="195" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A195">
         <v>2</v>
       </c>
@@ -9814,7 +9813,7 @@
         <v>1616</v>
       </c>
     </row>
-    <row r="196" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A196">
         <v>2</v>
       </c>
@@ -9834,7 +9833,7 @@
         <v>1696</v>
       </c>
     </row>
-    <row r="197" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A197">
         <v>2</v>
       </c>
@@ -9854,7 +9853,7 @@
         <v>1714</v>
       </c>
     </row>
-    <row r="198" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A198">
         <v>2</v>
       </c>
@@ -9874,7 +9873,7 @@
         <v>1728</v>
       </c>
     </row>
-    <row r="199" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A199">
         <v>2</v>
       </c>
@@ -9897,7 +9896,7 @@
         <v>1306</v>
       </c>
     </row>
-    <row r="200" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A200">
         <v>2</v>
       </c>
@@ -9917,7 +9916,7 @@
         <v>1741</v>
       </c>
     </row>
-    <row r="201" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A201">
         <v>2</v>
       </c>
@@ -9940,7 +9939,7 @@
         <v>1751</v>
       </c>
     </row>
-    <row r="202" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A202">
         <v>2</v>
       </c>
@@ -9960,7 +9959,7 @@
         <v>1755</v>
       </c>
     </row>
-    <row r="203" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A203">
         <v>2</v>
       </c>
@@ -9980,7 +9979,7 @@
         <v>1768</v>
       </c>
     </row>
-    <row r="204" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A204">
         <v>2</v>
       </c>
@@ -10000,7 +9999,7 @@
         <v>1806</v>
       </c>
     </row>
-    <row r="205" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A205">
         <v>2</v>
       </c>
@@ -10020,7 +10019,7 @@
         <v>1815</v>
       </c>
     </row>
-    <row r="206" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A206">
         <v>3</v>
       </c>
@@ -10040,7 +10039,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="207" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A207">
         <v>3</v>
       </c>
@@ -10060,7 +10059,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="208" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A208">
         <v>3</v>
       </c>
@@ -10080,7 +10079,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="209" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A209">
         <v>3</v>
       </c>
@@ -10100,7 +10099,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="210" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A210">
         <v>3</v>
       </c>
@@ -10120,7 +10119,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="211" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A211">
         <v>3</v>
       </c>
@@ -10140,7 +10139,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="212" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A212">
         <v>3</v>
       </c>
@@ -10160,7 +10159,7 @@
         <v>1049</v>
       </c>
     </row>
-    <row r="213" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A213">
         <v>3</v>
       </c>
@@ -10180,7 +10179,7 @@
         <v>1068</v>
       </c>
     </row>
-    <row r="214" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A214">
         <v>3</v>
       </c>
@@ -10200,7 +10199,7 @@
         <v>1737</v>
       </c>
     </row>
-    <row r="215" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A215">
         <v>3</v>
       </c>
@@ -10220,7 +10219,7 @@
         <v>1820</v>
       </c>
     </row>
-    <row r="216" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A216">
         <v>4</v>
       </c>
@@ -10240,7 +10239,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="217" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A217">
         <v>4</v>
       </c>
@@ -10263,7 +10262,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="218" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A218">
         <v>4</v>
       </c>
@@ -10286,7 +10285,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="219" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A219">
         <v>4</v>
       </c>
@@ -10306,7 +10305,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="220" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A220">
         <v>4</v>
       </c>
@@ -10329,7 +10328,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="221" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A221">
         <v>4</v>
       </c>
@@ -10352,7 +10351,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="222" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A222">
         <v>4</v>
       </c>
@@ -10375,7 +10374,7 @@
         <v>1149</v>
       </c>
     </row>
-    <row r="223" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A223">
         <v>4</v>
       </c>
@@ -10395,7 +10394,7 @@
         <v>1256</v>
       </c>
     </row>
-    <row r="224" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A224">
         <v>4</v>
       </c>
@@ -10418,7 +10417,7 @@
         <v>1287</v>
       </c>
     </row>
-    <row r="225" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A225">
         <v>4</v>
       </c>
@@ -10438,7 +10437,7 @@
         <v>1399</v>
       </c>
     </row>
-    <row r="226" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A226">
         <v>4</v>
       </c>
@@ -10458,7 +10457,7 @@
         <v>1574</v>
       </c>
     </row>
-    <row r="227" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A227">
         <v>4</v>
       </c>
@@ -13577,12 +13576,6 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:G379">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="UV"/>
-        <filter val="UV/HV"/>
-      </filters>
-    </filterColumn>
     <sortState ref="A2:G379">
       <sortCondition ref="A1:A379"/>
     </sortState>

</xml_diff>